<commit_message>
Add final table and slightly modify code+readme
</commit_message>
<xml_diff>
--- a/data/clean/Variables.xlsx
+++ b/data/clean/Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T450s\Desktop\programming\git\ba_da1\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BC5D8F-600A-42CC-A88C-575F224698EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC613A0A-85F2-4ED1-9A70-8AE09AFEC751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>Price in HUF</t>
   </si>
   <si>
-    <t>Name of Pizza</t>
-  </si>
-  <si>
     <t xml:space="preserve">No of customer ratings </t>
   </si>
   <si>
@@ -203,9 +200,6 @@
     </r>
   </si>
   <si>
-    <t>Size of Pizza in cm</t>
-  </si>
-  <si>
     <t>Address of restaurant</t>
   </si>
   <si>
@@ -213,6 +207,12 @@
   </si>
   <si>
     <t>Full address of restaurant inlcuding street,district,region, postal code, and city</t>
+  </si>
+  <si>
+    <t>Size of Pizza in cm or Beverage in l</t>
+  </si>
+  <si>
+    <t>Name of Pizza/Beverage</t>
   </si>
 </sst>
 </file>
@@ -282,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,17 +597,17 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.84375" customWidth="1"/>
-    <col min="2" max="2" width="10.53515625" customWidth="1"/>
-    <col min="3" max="3" width="104.3046875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="104.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -629,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -637,10 +637,10 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -659,10 +659,10 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -670,10 +670,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -681,10 +681,10 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -692,10 +692,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -703,10 +703,10 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -714,10 +714,10 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -725,10 +725,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -736,10 +736,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -747,10 +747,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -758,10 +758,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -769,10 +769,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -780,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add assignment csv with filtered variables
</commit_message>
<xml_diff>
--- a/data/clean/Variables.xlsx
+++ b/data/clean/Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T450s\Desktop\programming\git\ba_da1\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC613A0A-85F2-4ED1-9A70-8AE09AFEC751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C7EAD-6148-41FC-B6E0-604387CB8CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
+    <workbookView xWindow="25170" yWindow="-1590" windowWidth="21600" windowHeight="11385" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Variable</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Name of Pizza/Beverage</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concatenated string with max 5 tags available for a restaurant </t>
   </si>
 </sst>
 </file>
@@ -594,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95F57A2-06DD-4A37-A692-527DC5148D7D}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,6 +789,17 @@
         <v>33</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>